<commit_message>
add Healthz at backend
</commit_message>
<xml_diff>
--- a/Documentacao/EAP Sprint 1.xlsx
+++ b/Documentacao/EAP Sprint 1.xlsx
@@ -47,12 +47,6 @@
     <t>Lista de Pedidos Efetuados</t>
   </si>
   <si>
-    <t>Lista de Pedidos Entregues</t>
-  </si>
-  <si>
-    <t>Lista de Pedidos Pagos</t>
-  </si>
-  <si>
     <t>EAP - Sprint 1 - Projeto Loja Cupcakes</t>
   </si>
   <si>
@@ -117,6 +111,12 @@
   </si>
   <si>
     <t>1.7</t>
+  </si>
+  <si>
+    <t>Lista de Pedidos Pagos (através de Flag)</t>
+  </si>
+  <si>
+    <t>Lista de Pedidos Entregues (através de Flag)</t>
   </si>
 </sst>
 </file>
@@ -449,7 +449,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,7 +459,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -472,58 +472,58 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -536,7 +536,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -544,7 +544,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -552,7 +552,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>
@@ -560,7 +560,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -568,7 +568,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
@@ -576,18 +576,18 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>